<commit_message>
Remove spaces from words
</commit_message>
<xml_diff>
--- a/All_output.xlsx
+++ b/All_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="991">
   <si>
     <t>Nouns</t>
   </si>
@@ -103,7 +103,7 @@
     <t>highly</t>
   </si>
   <si>
-    <t xml:space="preserve"> cool</t>
+    <t>cool</t>
   </si>
   <si>
     <t>Around</t>
@@ -1153,9 +1153,6 @@
     <t>hot</t>
   </si>
   <si>
-    <t>cool</t>
-  </si>
-  <si>
     <t>quiet</t>
   </si>
   <si>
@@ -1921,7 +1918,7 @@
     <t>bottom</t>
   </si>
   <si>
-    <t xml:space="preserve">arrive </t>
+    <t>arrive</t>
   </si>
   <si>
     <t>sugar</t>
@@ -2008,7 +2005,7 @@
     <t>gray</t>
   </si>
   <si>
-    <t xml:space="preserve">sent  </t>
+    <t>sent</t>
   </si>
   <si>
     <t>fall</t>
@@ -5633,7 +5630,7 @@
         <v>66</v>
       </c>
       <c r="B94" t="s">
-        <v>379</v>
+        <v>29</v>
       </c>
       <c r="C94" t="s"/>
       <c r="D94" t="s"/>
@@ -5655,7 +5652,7 @@
         <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C95" t="s"/>
       <c r="D95" t="s"/>
@@ -5677,7 +5674,7 @@
         <v>86</v>
       </c>
       <c r="B96" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C96" t="s"/>
       <c r="D96" t="s"/>
@@ -5699,7 +5696,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C97" t="s"/>
       <c r="D97" t="s"/>
@@ -5721,7 +5718,7 @@
         <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C98" t="s"/>
       <c r="D98" t="s"/>
@@ -5743,7 +5740,7 @@
         <v>114</v>
       </c>
       <c r="B99" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C99" t="s"/>
       <c r="D99" t="s"/>
@@ -5762,10 +5759,10 @@
     </row>
     <row r="100" spans="1:14">
       <c r="A100" t="s">
+        <v>384</v>
+      </c>
+      <c r="B100" t="s">
         <v>385</v>
-      </c>
-      <c r="B100" t="s">
-        <v>386</v>
       </c>
       <c r="C100" t="s"/>
       <c r="D100" t="s"/>
@@ -5784,15 +5781,15 @@
     </row>
     <row r="101" spans="1:14">
       <c r="A101" t="s">
+        <v>386</v>
+      </c>
+      <c r="B101" t="s">
         <v>387</v>
-      </c>
-      <c r="B101" t="s">
-        <v>388</v>
       </c>
       <c r="C101" t="s"/>
       <c r="D101" t="s"/>
       <c r="E101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F101" t="s"/>
       <c r="G101" t="s"/>
@@ -5806,15 +5803,15 @@
     </row>
     <row r="102" spans="1:14">
       <c r="A102" t="s">
+        <v>389</v>
+      </c>
+      <c r="B102" t="s">
         <v>390</v>
-      </c>
-      <c r="B102" t="s">
-        <v>391</v>
       </c>
       <c r="C102" t="s"/>
       <c r="D102" t="s"/>
       <c r="E102" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F102" t="s"/>
       <c r="G102" t="s"/>
@@ -5828,15 +5825,15 @@
     </row>
     <row r="103" spans="1:14">
       <c r="A103" t="s">
+        <v>392</v>
+      </c>
+      <c r="B103" t="s">
         <v>393</v>
-      </c>
-      <c r="B103" t="s">
-        <v>394</v>
       </c>
       <c r="C103" t="s"/>
       <c r="D103" t="s"/>
       <c r="E103" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F103" t="s"/>
       <c r="G103" t="s"/>
@@ -5850,15 +5847,15 @@
     </row>
     <row r="104" spans="1:14">
       <c r="A104" t="s">
+        <v>395</v>
+      </c>
+      <c r="B104" t="s">
         <v>396</v>
-      </c>
-      <c r="B104" t="s">
-        <v>397</v>
       </c>
       <c r="C104" t="s"/>
       <c r="D104" t="s"/>
       <c r="E104" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F104" t="s"/>
       <c r="G104" t="s"/>
@@ -5872,15 +5869,15 @@
     </row>
     <row r="105" spans="1:14">
       <c r="A105" t="s">
+        <v>398</v>
+      </c>
+      <c r="B105" t="s">
         <v>399</v>
-      </c>
-      <c r="B105" t="s">
-        <v>400</v>
       </c>
       <c r="C105" t="s"/>
       <c r="D105" t="s"/>
       <c r="E105" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F105" t="s"/>
       <c r="G105" t="s"/>
@@ -5894,15 +5891,15 @@
     </row>
     <row r="106" spans="1:14">
       <c r="A106" t="s">
+        <v>401</v>
+      </c>
+      <c r="B106" t="s">
         <v>402</v>
-      </c>
-      <c r="B106" t="s">
-        <v>403</v>
       </c>
       <c r="C106" t="s"/>
       <c r="D106" t="s"/>
       <c r="E106" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F106" t="s"/>
       <c r="G106" t="s"/>
@@ -5916,15 +5913,15 @@
     </row>
     <row r="107" spans="1:14">
       <c r="A107" t="s">
+        <v>404</v>
+      </c>
+      <c r="B107" t="s">
         <v>405</v>
-      </c>
-      <c r="B107" t="s">
-        <v>406</v>
       </c>
       <c r="C107" t="s"/>
       <c r="D107" t="s"/>
       <c r="E107" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F107" t="s"/>
       <c r="G107" t="s"/>
@@ -5938,15 +5935,15 @@
     </row>
     <row r="108" spans="1:14">
       <c r="A108" t="s">
+        <v>407</v>
+      </c>
+      <c r="B108" t="s">
         <v>408</v>
-      </c>
-      <c r="B108" t="s">
-        <v>409</v>
       </c>
       <c r="C108" t="s"/>
       <c r="D108" t="s"/>
       <c r="E108" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F108" t="s"/>
       <c r="G108" t="s"/>
@@ -5960,15 +5957,15 @@
     </row>
     <row r="109" spans="1:14">
       <c r="A109" t="s">
+        <v>410</v>
+      </c>
+      <c r="B109" t="s">
         <v>411</v>
-      </c>
-      <c r="B109" t="s">
-        <v>412</v>
       </c>
       <c r="C109" t="s"/>
       <c r="D109" t="s"/>
       <c r="E109" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F109" t="s"/>
       <c r="G109" t="s"/>
@@ -5982,15 +5979,15 @@
     </row>
     <row r="110" spans="1:14">
       <c r="A110" t="s">
+        <v>413</v>
+      </c>
+      <c r="B110" t="s">
         <v>414</v>
-      </c>
-      <c r="B110" t="s">
-        <v>415</v>
       </c>
       <c r="C110" t="s"/>
       <c r="D110" t="s"/>
       <c r="E110" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F110" t="s"/>
       <c r="G110" t="s"/>
@@ -6004,15 +6001,15 @@
     </row>
     <row r="111" spans="1:14">
       <c r="A111" t="s">
+        <v>416</v>
+      </c>
+      <c r="B111" t="s">
         <v>417</v>
-      </c>
-      <c r="B111" t="s">
-        <v>418</v>
       </c>
       <c r="C111" t="s"/>
       <c r="D111" t="s"/>
       <c r="E111" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="F111" t="s"/>
       <c r="G111" t="s"/>
@@ -6026,15 +6023,15 @@
     </row>
     <row r="112" spans="1:14">
       <c r="A112" t="s">
+        <v>419</v>
+      </c>
+      <c r="B112" t="s">
         <v>420</v>
-      </c>
-      <c r="B112" t="s">
-        <v>421</v>
       </c>
       <c r="C112" t="s"/>
       <c r="D112" t="s"/>
       <c r="E112" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F112" t="s"/>
       <c r="G112" t="s"/>
@@ -6048,15 +6045,15 @@
     </row>
     <row r="113" spans="1:14">
       <c r="A113" t="s">
+        <v>422</v>
+      </c>
+      <c r="B113" t="s">
         <v>423</v>
-      </c>
-      <c r="B113" t="s">
-        <v>424</v>
       </c>
       <c r="C113" t="s"/>
       <c r="D113" t="s"/>
       <c r="E113" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F113" t="s"/>
       <c r="G113" t="s"/>
@@ -6070,15 +6067,15 @@
     </row>
     <row r="114" spans="1:14">
       <c r="A114" t="s">
+        <v>425</v>
+      </c>
+      <c r="B114" t="s">
         <v>426</v>
-      </c>
-      <c r="B114" t="s">
-        <v>427</v>
       </c>
       <c r="C114" t="s"/>
       <c r="D114" t="s"/>
       <c r="E114" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F114" t="s"/>
       <c r="G114" t="s"/>
@@ -6092,15 +6089,15 @@
     </row>
     <row r="115" spans="1:14">
       <c r="A115" t="s">
+        <v>428</v>
+      </c>
+      <c r="B115" t="s">
         <v>429</v>
-      </c>
-      <c r="B115" t="s">
-        <v>430</v>
       </c>
       <c r="C115" t="s"/>
       <c r="D115" t="s"/>
       <c r="E115" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F115" t="s"/>
       <c r="G115" t="s"/>
@@ -6114,15 +6111,15 @@
     </row>
     <row r="116" spans="1:14">
       <c r="A116" t="s">
+        <v>431</v>
+      </c>
+      <c r="B116" t="s">
         <v>432</v>
-      </c>
-      <c r="B116" t="s">
-        <v>433</v>
       </c>
       <c r="C116" t="s"/>
       <c r="D116" t="s"/>
       <c r="E116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F116" t="s"/>
       <c r="G116" t="s"/>
@@ -6136,15 +6133,15 @@
     </row>
     <row r="117" spans="1:14">
       <c r="A117" t="s">
+        <v>434</v>
+      </c>
+      <c r="B117" t="s">
         <v>435</v>
-      </c>
-      <c r="B117" t="s">
-        <v>436</v>
       </c>
       <c r="C117" t="s"/>
       <c r="D117" t="s"/>
       <c r="E117" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F117" t="s"/>
       <c r="G117" t="s"/>
@@ -6158,15 +6155,15 @@
     </row>
     <row r="118" spans="1:14">
       <c r="A118" t="s">
+        <v>437</v>
+      </c>
+      <c r="B118" t="s">
         <v>438</v>
-      </c>
-      <c r="B118" t="s">
-        <v>439</v>
       </c>
       <c r="C118" t="s"/>
       <c r="D118" t="s"/>
       <c r="E118" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F118" t="s"/>
       <c r="G118" t="s"/>
@@ -6180,15 +6177,15 @@
     </row>
     <row r="119" spans="1:14">
       <c r="A119" t="s">
+        <v>440</v>
+      </c>
+      <c r="B119" t="s">
         <v>441</v>
-      </c>
-      <c r="B119" t="s">
-        <v>442</v>
       </c>
       <c r="C119" t="s"/>
       <c r="D119" t="s"/>
       <c r="E119" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F119" t="s"/>
       <c r="G119" t="s"/>
@@ -6202,15 +6199,15 @@
     </row>
     <row r="120" spans="1:14">
       <c r="A120" t="s">
+        <v>443</v>
+      </c>
+      <c r="B120" t="s">
         <v>444</v>
-      </c>
-      <c r="B120" t="s">
-        <v>445</v>
       </c>
       <c r="C120" t="s"/>
       <c r="D120" t="s"/>
       <c r="E120" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F120" t="s"/>
       <c r="G120" t="s"/>
@@ -6224,15 +6221,15 @@
     </row>
     <row r="121" spans="1:14">
       <c r="A121" t="s">
+        <v>446</v>
+      </c>
+      <c r="B121" t="s">
         <v>447</v>
-      </c>
-      <c r="B121" t="s">
-        <v>448</v>
       </c>
       <c r="C121" t="s"/>
       <c r="D121" t="s"/>
       <c r="E121" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F121" t="s"/>
       <c r="G121" t="s"/>
@@ -6246,7 +6243,7 @@
     </row>
     <row r="122" spans="1:14">
       <c r="A122" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B122" t="s">
         <v>342</v>
@@ -6254,7 +6251,7 @@
       <c r="C122" t="s"/>
       <c r="D122" t="s"/>
       <c r="E122" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F122" t="s"/>
       <c r="G122" t="s"/>
@@ -6268,15 +6265,15 @@
     </row>
     <row r="123" spans="1:14">
       <c r="A123" t="s">
+        <v>451</v>
+      </c>
+      <c r="B123" t="s">
         <v>452</v>
-      </c>
-      <c r="B123" t="s">
-        <v>453</v>
       </c>
       <c r="C123" t="s"/>
       <c r="D123" t="s"/>
       <c r="E123" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F123" t="s"/>
       <c r="G123" t="s"/>
@@ -6290,15 +6287,15 @@
     </row>
     <row r="124" spans="1:14">
       <c r="A124" t="s">
+        <v>454</v>
+      </c>
+      <c r="B124" t="s">
         <v>455</v>
-      </c>
-      <c r="B124" t="s">
-        <v>456</v>
       </c>
       <c r="C124" t="s"/>
       <c r="D124" t="s"/>
       <c r="E124" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F124" t="s"/>
       <c r="G124" t="s"/>
@@ -6312,15 +6309,15 @@
     </row>
     <row r="125" spans="1:14">
       <c r="A125" t="s">
+        <v>457</v>
+      </c>
+      <c r="B125" t="s">
         <v>458</v>
-      </c>
-      <c r="B125" t="s">
-        <v>459</v>
       </c>
       <c r="C125" t="s"/>
       <c r="D125" t="s"/>
       <c r="E125" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F125" t="s"/>
       <c r="G125" t="s"/>
@@ -6334,15 +6331,15 @@
     </row>
     <row r="126" spans="1:14">
       <c r="A126" t="s">
+        <v>460</v>
+      </c>
+      <c r="B126" t="s">
         <v>461</v>
-      </c>
-      <c r="B126" t="s">
-        <v>462</v>
       </c>
       <c r="C126" t="s"/>
       <c r="D126" t="s"/>
       <c r="E126" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F126" t="s"/>
       <c r="G126" t="s"/>
@@ -6356,15 +6353,15 @@
     </row>
     <row r="127" spans="1:14">
       <c r="A127" t="s">
+        <v>463</v>
+      </c>
+      <c r="B127" t="s">
         <v>464</v>
-      </c>
-      <c r="B127" t="s">
-        <v>465</v>
       </c>
       <c r="C127" t="s"/>
       <c r="D127" t="s"/>
       <c r="E127" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F127" t="s"/>
       <c r="G127" t="s"/>
@@ -6378,15 +6375,15 @@
     </row>
     <row r="128" spans="1:14">
       <c r="A128" t="s">
+        <v>466</v>
+      </c>
+      <c r="B128" t="s">
         <v>467</v>
-      </c>
-      <c r="B128" t="s">
-        <v>468</v>
       </c>
       <c r="C128" t="s"/>
       <c r="D128" t="s"/>
       <c r="E128" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F128" t="s"/>
       <c r="G128" t="s"/>
@@ -6400,15 +6397,15 @@
     </row>
     <row r="129" spans="1:14">
       <c r="A129" t="s">
+        <v>469</v>
+      </c>
+      <c r="B129" t="s">
         <v>470</v>
-      </c>
-      <c r="B129" t="s">
-        <v>471</v>
       </c>
       <c r="C129" t="s"/>
       <c r="D129" t="s"/>
       <c r="E129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F129" t="s"/>
       <c r="G129" t="s"/>
@@ -6422,15 +6419,15 @@
     </row>
     <row r="130" spans="1:14">
       <c r="A130" t="s">
+        <v>472</v>
+      </c>
+      <c r="B130" t="s">
         <v>473</v>
-      </c>
-      <c r="B130" t="s">
-        <v>474</v>
       </c>
       <c r="C130" t="s"/>
       <c r="D130" t="s"/>
       <c r="E130" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F130" t="s"/>
       <c r="G130" t="s"/>
@@ -6444,15 +6441,15 @@
     </row>
     <row r="131" spans="1:14">
       <c r="A131" t="s">
+        <v>475</v>
+      </c>
+      <c r="B131" t="s">
         <v>476</v>
-      </c>
-      <c r="B131" t="s">
-        <v>477</v>
       </c>
       <c r="C131" t="s"/>
       <c r="D131" t="s"/>
       <c r="E131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F131" t="s"/>
       <c r="G131" t="s"/>
@@ -6466,7 +6463,7 @@
     </row>
     <row r="132" spans="1:14">
       <c r="A132" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B132" t="b">
         <v>1</v>
@@ -6474,7 +6471,7 @@
       <c r="C132" t="s"/>
       <c r="D132" t="s"/>
       <c r="E132" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F132" t="s"/>
       <c r="G132" t="s"/>
@@ -6488,15 +6485,15 @@
     </row>
     <row r="133" spans="1:14">
       <c r="A133" t="s">
+        <v>480</v>
+      </c>
+      <c r="B133" t="s">
         <v>481</v>
-      </c>
-      <c r="B133" t="s">
-        <v>482</v>
       </c>
       <c r="C133" t="s"/>
       <c r="D133" t="s"/>
       <c r="E133" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F133" t="s"/>
       <c r="G133" t="s"/>
@@ -6510,15 +6507,15 @@
     </row>
     <row r="134" spans="1:14">
       <c r="A134" t="s">
+        <v>483</v>
+      </c>
+      <c r="B134" t="s">
         <v>484</v>
-      </c>
-      <c r="B134" t="s">
-        <v>485</v>
       </c>
       <c r="C134" t="s"/>
       <c r="D134" t="s"/>
       <c r="E134" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F134" t="s"/>
       <c r="G134" t="s"/>
@@ -6532,15 +6529,15 @@
     </row>
     <row r="135" spans="1:14">
       <c r="A135" t="s">
+        <v>486</v>
+      </c>
+      <c r="B135" t="s">
         <v>487</v>
-      </c>
-      <c r="B135" t="s">
-        <v>488</v>
       </c>
       <c r="C135" t="s"/>
       <c r="D135" t="s"/>
       <c r="E135" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F135" t="s"/>
       <c r="G135" t="s"/>
@@ -6554,15 +6551,15 @@
     </row>
     <row r="136" spans="1:14">
       <c r="A136" t="s">
+        <v>489</v>
+      </c>
+      <c r="B136" t="s">
         <v>490</v>
-      </c>
-      <c r="B136" t="s">
-        <v>491</v>
       </c>
       <c r="C136" t="s"/>
       <c r="D136" t="s"/>
       <c r="E136" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F136" t="s"/>
       <c r="G136" t="s"/>
@@ -6576,15 +6573,15 @@
     </row>
     <row r="137" spans="1:14">
       <c r="A137" t="s">
+        <v>492</v>
+      </c>
+      <c r="B137" t="s">
         <v>493</v>
-      </c>
-      <c r="B137" t="s">
-        <v>494</v>
       </c>
       <c r="C137" t="s"/>
       <c r="D137" t="s"/>
       <c r="E137" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F137" t="s"/>
       <c r="G137" t="s"/>
@@ -6598,15 +6595,15 @@
     </row>
     <row r="138" spans="1:14">
       <c r="A138" t="s">
+        <v>495</v>
+      </c>
+      <c r="B138" t="s">
         <v>496</v>
-      </c>
-      <c r="B138" t="s">
-        <v>497</v>
       </c>
       <c r="C138" t="s"/>
       <c r="D138" t="s"/>
       <c r="E138" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F138" t="s"/>
       <c r="G138" t="s"/>
@@ -6620,15 +6617,15 @@
     </row>
     <row r="139" spans="1:14">
       <c r="A139" t="s">
+        <v>498</v>
+      </c>
+      <c r="B139" t="s">
         <v>499</v>
-      </c>
-      <c r="B139" t="s">
-        <v>500</v>
       </c>
       <c r="C139" t="s"/>
       <c r="D139" t="s"/>
       <c r="E139" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F139" t="s"/>
       <c r="G139" t="s"/>
@@ -6642,15 +6639,15 @@
     </row>
     <row r="140" spans="1:14">
       <c r="A140" t="s">
+        <v>501</v>
+      </c>
+      <c r="B140" t="s">
         <v>502</v>
-      </c>
-      <c r="B140" t="s">
-        <v>503</v>
       </c>
       <c r="C140" t="s"/>
       <c r="D140" t="s"/>
       <c r="E140" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F140" t="s"/>
       <c r="G140" t="s"/>
@@ -6664,15 +6661,15 @@
     </row>
     <row r="141" spans="1:14">
       <c r="A141" t="s">
+        <v>504</v>
+      </c>
+      <c r="B141" t="s">
         <v>505</v>
-      </c>
-      <c r="B141" t="s">
-        <v>506</v>
       </c>
       <c r="C141" t="s"/>
       <c r="D141" t="s"/>
       <c r="E141" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F141" t="s"/>
       <c r="G141" t="s"/>
@@ -6686,15 +6683,15 @@
     </row>
     <row r="142" spans="1:14">
       <c r="A142" t="s">
+        <v>507</v>
+      </c>
+      <c r="B142" t="s">
         <v>508</v>
-      </c>
-      <c r="B142" t="s">
-        <v>509</v>
       </c>
       <c r="C142" t="s"/>
       <c r="D142" t="s"/>
       <c r="E142" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F142" t="s"/>
       <c r="G142" t="s"/>
@@ -6708,15 +6705,15 @@
     </row>
     <row r="143" spans="1:14">
       <c r="A143" t="s">
+        <v>509</v>
+      </c>
+      <c r="B143" t="s">
         <v>510</v>
-      </c>
-      <c r="B143" t="s">
-        <v>511</v>
       </c>
       <c r="C143" t="s"/>
       <c r="D143" t="s"/>
       <c r="E143" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F143" t="s"/>
       <c r="G143" t="s"/>
@@ -6730,15 +6727,15 @@
     </row>
     <row r="144" spans="1:14">
       <c r="A144" t="s">
+        <v>512</v>
+      </c>
+      <c r="B144" t="s">
         <v>513</v>
-      </c>
-      <c r="B144" t="s">
-        <v>514</v>
       </c>
       <c r="C144" t="s"/>
       <c r="D144" t="s"/>
       <c r="E144" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F144" t="s"/>
       <c r="G144" t="s"/>
@@ -6752,15 +6749,15 @@
     </row>
     <row r="145" spans="1:14">
       <c r="A145" t="s">
+        <v>515</v>
+      </c>
+      <c r="B145" t="s">
         <v>516</v>
-      </c>
-      <c r="B145" t="s">
-        <v>517</v>
       </c>
       <c r="C145" t="s"/>
       <c r="D145" t="s"/>
       <c r="E145" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F145" t="s"/>
       <c r="G145" t="s"/>
@@ -6774,15 +6771,15 @@
     </row>
     <row r="146" spans="1:14">
       <c r="A146" t="s">
+        <v>518</v>
+      </c>
+      <c r="B146" t="s">
         <v>519</v>
-      </c>
-      <c r="B146" t="s">
-        <v>520</v>
       </c>
       <c r="C146" t="s"/>
       <c r="D146" t="s"/>
       <c r="E146" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F146" t="s"/>
       <c r="G146" t="s"/>
@@ -6796,15 +6793,15 @@
     </row>
     <row r="147" spans="1:14">
       <c r="A147" t="s">
+        <v>521</v>
+      </c>
+      <c r="B147" t="s">
         <v>522</v>
-      </c>
-      <c r="B147" t="s">
-        <v>523</v>
       </c>
       <c r="C147" t="s"/>
       <c r="D147" t="s"/>
       <c r="E147" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F147" t="s"/>
       <c r="G147" t="s"/>
@@ -6818,15 +6815,15 @@
     </row>
     <row r="148" spans="1:14">
       <c r="A148" t="s">
+        <v>524</v>
+      </c>
+      <c r="B148" t="s">
         <v>525</v>
-      </c>
-      <c r="B148" t="s">
-        <v>526</v>
       </c>
       <c r="C148" t="s"/>
       <c r="D148" t="s"/>
       <c r="E148" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F148" t="s"/>
       <c r="G148" t="s"/>
@@ -6840,15 +6837,15 @@
     </row>
     <row r="149" spans="1:14">
       <c r="A149" t="s">
+        <v>527</v>
+      </c>
+      <c r="B149" t="s">
         <v>528</v>
-      </c>
-      <c r="B149" t="s">
-        <v>529</v>
       </c>
       <c r="C149" t="s"/>
       <c r="D149" t="s"/>
       <c r="E149" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F149" t="s"/>
       <c r="G149" t="s"/>
@@ -6862,15 +6859,15 @@
     </row>
     <row r="150" spans="1:14">
       <c r="A150" t="s">
+        <v>530</v>
+      </c>
+      <c r="B150" t="s">
         <v>531</v>
-      </c>
-      <c r="B150" t="s">
-        <v>532</v>
       </c>
       <c r="C150" t="s"/>
       <c r="D150" t="s"/>
       <c r="E150" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F150" t="s"/>
       <c r="G150" t="s"/>
@@ -6884,15 +6881,15 @@
     </row>
     <row r="151" spans="1:14">
       <c r="A151" t="s">
+        <v>533</v>
+      </c>
+      <c r="B151" t="s">
         <v>534</v>
-      </c>
-      <c r="B151" t="s">
-        <v>535</v>
       </c>
       <c r="C151" t="s"/>
       <c r="D151" t="s"/>
       <c r="E151" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F151" t="s"/>
       <c r="G151" t="s"/>
@@ -6906,15 +6903,15 @@
     </row>
     <row r="152" spans="1:14">
       <c r="A152" t="s">
+        <v>536</v>
+      </c>
+      <c r="B152" t="s">
         <v>537</v>
-      </c>
-      <c r="B152" t="s">
-        <v>538</v>
       </c>
       <c r="C152" t="s"/>
       <c r="D152" t="s"/>
       <c r="E152" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F152" t="s"/>
       <c r="G152" t="s"/>
@@ -6928,15 +6925,15 @@
     </row>
     <row r="153" spans="1:14">
       <c r="A153" t="s">
+        <v>539</v>
+      </c>
+      <c r="B153" t="s">
         <v>540</v>
-      </c>
-      <c r="B153" t="s">
-        <v>541</v>
       </c>
       <c r="C153" t="s"/>
       <c r="D153" t="s"/>
       <c r="E153" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F153" t="s"/>
       <c r="G153" t="s"/>
@@ -6950,15 +6947,15 @@
     </row>
     <row r="154" spans="1:14">
       <c r="A154" t="s">
+        <v>542</v>
+      </c>
+      <c r="B154" t="s">
         <v>543</v>
-      </c>
-      <c r="B154" t="s">
-        <v>544</v>
       </c>
       <c r="C154" t="s"/>
       <c r="D154" t="s"/>
       <c r="E154" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F154" t="s"/>
       <c r="G154" t="s"/>
@@ -6972,15 +6969,15 @@
     </row>
     <row r="155" spans="1:14">
       <c r="A155" t="s">
+        <v>545</v>
+      </c>
+      <c r="B155" t="s">
         <v>546</v>
-      </c>
-      <c r="B155" t="s">
-        <v>547</v>
       </c>
       <c r="C155" t="s"/>
       <c r="D155" t="s"/>
       <c r="E155" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F155" t="s"/>
       <c r="G155" t="s"/>
@@ -6994,15 +6991,15 @@
     </row>
     <row r="156" spans="1:14">
       <c r="A156" t="s">
+        <v>548</v>
+      </c>
+      <c r="B156" t="s">
         <v>549</v>
-      </c>
-      <c r="B156" t="s">
-        <v>550</v>
       </c>
       <c r="C156" t="s"/>
       <c r="D156" t="s"/>
       <c r="E156" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F156" t="s"/>
       <c r="G156" t="s"/>
@@ -7016,15 +7013,15 @@
     </row>
     <row r="157" spans="1:14">
       <c r="A157" t="s">
+        <v>551</v>
+      </c>
+      <c r="B157" t="s">
         <v>552</v>
-      </c>
-      <c r="B157" t="s">
-        <v>553</v>
       </c>
       <c r="C157" t="s"/>
       <c r="D157" t="s"/>
       <c r="E157" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F157" t="s"/>
       <c r="G157" t="s"/>
@@ -7038,7 +7035,7 @@
     </row>
     <row r="158" spans="1:14">
       <c r="A158" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B158" t="s">
         <v>94</v>
@@ -7046,7 +7043,7 @@
       <c r="C158" t="s"/>
       <c r="D158" t="s"/>
       <c r="E158" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F158" t="s"/>
       <c r="G158" t="s"/>
@@ -7060,15 +7057,15 @@
     </row>
     <row r="159" spans="1:14">
       <c r="A159" t="s">
+        <v>556</v>
+      </c>
+      <c r="B159" t="s">
         <v>557</v>
-      </c>
-      <c r="B159" t="s">
-        <v>558</v>
       </c>
       <c r="C159" t="s"/>
       <c r="D159" t="s"/>
       <c r="E159" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F159" t="s"/>
       <c r="G159" t="s"/>
@@ -7082,15 +7079,15 @@
     </row>
     <row r="160" spans="1:14">
       <c r="A160" t="s">
+        <v>559</v>
+      </c>
+      <c r="B160" t="s">
         <v>560</v>
-      </c>
-      <c r="B160" t="s">
-        <v>561</v>
       </c>
       <c r="C160" t="s"/>
       <c r="D160" t="s"/>
       <c r="E160" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F160" t="s"/>
       <c r="G160" t="s"/>
@@ -7104,15 +7101,15 @@
     </row>
     <row r="161" spans="1:14">
       <c r="A161" t="s">
+        <v>562</v>
+      </c>
+      <c r="B161" t="s">
         <v>563</v>
-      </c>
-      <c r="B161" t="s">
-        <v>564</v>
       </c>
       <c r="C161" t="s"/>
       <c r="D161" t="s"/>
       <c r="E161" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F161" t="s"/>
       <c r="G161" t="s"/>
@@ -7126,15 +7123,15 @@
     </row>
     <row r="162" spans="1:14">
       <c r="A162" t="s">
+        <v>565</v>
+      </c>
+      <c r="B162" t="s">
         <v>566</v>
-      </c>
-      <c r="B162" t="s">
-        <v>567</v>
       </c>
       <c r="C162" t="s"/>
       <c r="D162" t="s"/>
       <c r="E162" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F162" t="s"/>
       <c r="G162" t="s"/>
@@ -7148,15 +7145,15 @@
     </row>
     <row r="163" spans="1:14">
       <c r="A163" t="s">
+        <v>568</v>
+      </c>
+      <c r="B163" t="s">
         <v>569</v>
-      </c>
-      <c r="B163" t="s">
-        <v>570</v>
       </c>
       <c r="C163" t="s"/>
       <c r="D163" t="s"/>
       <c r="E163" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F163" t="s"/>
       <c r="G163" t="s"/>
@@ -7170,15 +7167,15 @@
     </row>
     <row r="164" spans="1:14">
       <c r="A164" t="s">
+        <v>571</v>
+      </c>
+      <c r="B164" t="s">
         <v>572</v>
-      </c>
-      <c r="B164" t="s">
-        <v>573</v>
       </c>
       <c r="C164" t="s"/>
       <c r="D164" t="s"/>
       <c r="E164" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F164" t="s"/>
       <c r="G164" t="s"/>
@@ -7192,15 +7189,15 @@
     </row>
     <row r="165" spans="1:14">
       <c r="A165" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B165" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C165" t="s"/>
       <c r="D165" t="s"/>
       <c r="E165" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F165" t="s"/>
       <c r="G165" t="s"/>
@@ -7214,15 +7211,15 @@
     </row>
     <row r="166" spans="1:14">
       <c r="A166" t="s">
+        <v>576</v>
+      </c>
+      <c r="B166" t="s">
         <v>577</v>
-      </c>
-      <c r="B166" t="s">
-        <v>578</v>
       </c>
       <c r="C166" t="s"/>
       <c r="D166" t="s"/>
       <c r="E166" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F166" t="s"/>
       <c r="G166" t="s"/>
@@ -7236,15 +7233,15 @@
     </row>
     <row r="167" spans="1:14">
       <c r="A167" t="s">
+        <v>579</v>
+      </c>
+      <c r="B167" t="s">
         <v>580</v>
-      </c>
-      <c r="B167" t="s">
-        <v>581</v>
       </c>
       <c r="C167" t="s"/>
       <c r="D167" t="s"/>
       <c r="E167" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F167" t="s"/>
       <c r="G167" t="s"/>
@@ -7258,15 +7255,15 @@
     </row>
     <row r="168" spans="1:14">
       <c r="A168" t="s">
+        <v>582</v>
+      </c>
+      <c r="B168" t="s">
         <v>583</v>
-      </c>
-      <c r="B168" t="s">
-        <v>584</v>
       </c>
       <c r="C168" t="s"/>
       <c r="D168" t="s"/>
       <c r="E168" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F168" t="s"/>
       <c r="G168" t="s"/>
@@ -7280,15 +7277,15 @@
     </row>
     <row r="169" spans="1:14">
       <c r="A169" t="s">
+        <v>585</v>
+      </c>
+      <c r="B169" t="s">
         <v>586</v>
-      </c>
-      <c r="B169" t="s">
-        <v>587</v>
       </c>
       <c r="C169" t="s"/>
       <c r="D169" t="s"/>
       <c r="E169" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F169" t="s"/>
       <c r="G169" t="s"/>
@@ -7302,15 +7299,15 @@
     </row>
     <row r="170" spans="1:14">
       <c r="A170" t="s">
+        <v>588</v>
+      </c>
+      <c r="B170" t="s">
         <v>589</v>
-      </c>
-      <c r="B170" t="s">
-        <v>590</v>
       </c>
       <c r="C170" t="s"/>
       <c r="D170" t="s"/>
       <c r="E170" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F170" t="s"/>
       <c r="G170" t="s"/>
@@ -7324,15 +7321,15 @@
     </row>
     <row r="171" spans="1:14">
       <c r="A171" t="s">
+        <v>591</v>
+      </c>
+      <c r="B171" t="s">
         <v>592</v>
-      </c>
-      <c r="B171" t="s">
-        <v>593</v>
       </c>
       <c r="C171" t="s"/>
       <c r="D171" t="s"/>
       <c r="E171" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F171" t="s"/>
       <c r="G171" t="s"/>
@@ -7346,15 +7343,15 @@
     </row>
     <row r="172" spans="1:14">
       <c r="A172" t="s">
+        <v>594</v>
+      </c>
+      <c r="B172" t="s">
         <v>595</v>
-      </c>
-      <c r="B172" t="s">
-        <v>596</v>
       </c>
       <c r="C172" t="s"/>
       <c r="D172" t="s"/>
       <c r="E172" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F172" t="s"/>
       <c r="G172" t="s"/>
@@ -7368,15 +7365,15 @@
     </row>
     <row r="173" spans="1:14">
       <c r="A173" t="s">
+        <v>597</v>
+      </c>
+      <c r="B173" t="s">
         <v>598</v>
-      </c>
-      <c r="B173" t="s">
-        <v>599</v>
       </c>
       <c r="C173" t="s"/>
       <c r="D173" t="s"/>
       <c r="E173" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F173" t="s"/>
       <c r="G173" t="s"/>
@@ -7390,15 +7387,15 @@
     </row>
     <row r="174" spans="1:14">
       <c r="A174" t="s">
+        <v>600</v>
+      </c>
+      <c r="B174" t="s">
         <v>601</v>
-      </c>
-      <c r="B174" t="s">
-        <v>602</v>
       </c>
       <c r="C174" t="s"/>
       <c r="D174" t="s"/>
       <c r="E174" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F174" t="s"/>
       <c r="G174" t="s"/>
@@ -7412,15 +7409,15 @@
     </row>
     <row r="175" spans="1:14">
       <c r="A175" t="s">
+        <v>603</v>
+      </c>
+      <c r="B175" t="s">
         <v>604</v>
-      </c>
-      <c r="B175" t="s">
-        <v>605</v>
       </c>
       <c r="C175" t="s"/>
       <c r="D175" t="s"/>
       <c r="E175" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F175" t="s"/>
       <c r="G175" t="s"/>
@@ -7434,15 +7431,15 @@
     </row>
     <row r="176" spans="1:14">
       <c r="A176" t="s">
+        <v>606</v>
+      </c>
+      <c r="B176" t="s">
         <v>607</v>
-      </c>
-      <c r="B176" t="s">
-        <v>608</v>
       </c>
       <c r="C176" t="s"/>
       <c r="D176" t="s"/>
       <c r="E176" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F176" t="s"/>
       <c r="G176" t="s"/>
@@ -7456,15 +7453,15 @@
     </row>
     <row r="177" spans="1:14">
       <c r="A177" t="s">
+        <v>609</v>
+      </c>
+      <c r="B177" t="s">
         <v>610</v>
-      </c>
-      <c r="B177" t="s">
-        <v>611</v>
       </c>
       <c r="C177" t="s"/>
       <c r="D177" t="s"/>
       <c r="E177" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F177" t="s"/>
       <c r="G177" t="s"/>
@@ -7478,15 +7475,15 @@
     </row>
     <row r="178" spans="1:14">
       <c r="A178" t="s">
+        <v>612</v>
+      </c>
+      <c r="B178" t="s">
         <v>613</v>
-      </c>
-      <c r="B178" t="s">
-        <v>614</v>
       </c>
       <c r="C178" t="s"/>
       <c r="D178" t="s"/>
       <c r="E178" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F178" t="s"/>
       <c r="G178" t="s"/>
@@ -7500,15 +7497,15 @@
     </row>
     <row r="179" spans="1:14">
       <c r="A179" t="s">
+        <v>615</v>
+      </c>
+      <c r="B179" t="s">
         <v>616</v>
-      </c>
-      <c r="B179" t="s">
-        <v>617</v>
       </c>
       <c r="C179" t="s"/>
       <c r="D179" t="s"/>
       <c r="E179" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F179" t="s"/>
       <c r="G179" t="s"/>
@@ -7522,15 +7519,15 @@
     </row>
     <row r="180" spans="1:14">
       <c r="A180" t="s">
+        <v>618</v>
+      </c>
+      <c r="B180" t="s">
         <v>619</v>
-      </c>
-      <c r="B180" t="s">
-        <v>620</v>
       </c>
       <c r="C180" t="s"/>
       <c r="D180" t="s"/>
       <c r="E180" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F180" t="s"/>
       <c r="G180" t="s"/>
@@ -7544,15 +7541,15 @@
     </row>
     <row r="181" spans="1:14">
       <c r="A181" t="s">
+        <v>621</v>
+      </c>
+      <c r="B181" t="s">
         <v>622</v>
-      </c>
-      <c r="B181" t="s">
-        <v>623</v>
       </c>
       <c r="C181" t="s"/>
       <c r="D181" t="s"/>
       <c r="E181" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F181" t="s"/>
       <c r="G181" t="s"/>
@@ -7566,15 +7563,15 @@
     </row>
     <row r="182" spans="1:14">
       <c r="A182" t="s">
+        <v>624</v>
+      </c>
+      <c r="B182" t="s">
         <v>625</v>
-      </c>
-      <c r="B182" t="s">
-        <v>626</v>
       </c>
       <c r="C182" t="s"/>
       <c r="D182" t="s"/>
       <c r="E182" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F182" t="s"/>
       <c r="G182" t="s"/>
@@ -7588,15 +7585,15 @@
     </row>
     <row r="183" spans="1:14">
       <c r="A183" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B183" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C183" t="s"/>
       <c r="D183" t="s"/>
       <c r="E183" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F183" t="s"/>
       <c r="G183" t="s"/>
@@ -7610,15 +7607,15 @@
     </row>
     <row r="184" spans="1:14">
       <c r="A184" t="s">
+        <v>629</v>
+      </c>
+      <c r="B184" t="s">
         <v>630</v>
-      </c>
-      <c r="B184" t="s">
-        <v>631</v>
       </c>
       <c r="C184" t="s"/>
       <c r="D184" t="s"/>
       <c r="E184" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F184" t="s"/>
       <c r="G184" t="s"/>
@@ -7632,15 +7629,15 @@
     </row>
     <row r="185" spans="1:14">
       <c r="A185" t="s">
+        <v>632</v>
+      </c>
+      <c r="B185" t="s">
         <v>633</v>
-      </c>
-      <c r="B185" t="s">
-        <v>634</v>
       </c>
       <c r="C185" t="s"/>
       <c r="D185" t="s"/>
       <c r="E185" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F185" t="s"/>
       <c r="G185" t="s"/>
@@ -7654,15 +7651,15 @@
     </row>
     <row r="186" spans="1:14">
       <c r="A186" t="s">
+        <v>635</v>
+      </c>
+      <c r="B186" t="s">
         <v>636</v>
-      </c>
-      <c r="B186" t="s">
-        <v>637</v>
       </c>
       <c r="C186" t="s"/>
       <c r="D186" t="s"/>
       <c r="E186" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F186" t="s"/>
       <c r="G186" t="s"/>
@@ -7676,15 +7673,15 @@
     </row>
     <row r="187" spans="1:14">
       <c r="A187" t="s">
+        <v>638</v>
+      </c>
+      <c r="B187" t="s">
         <v>639</v>
-      </c>
-      <c r="B187" t="s">
-        <v>640</v>
       </c>
       <c r="C187" t="s"/>
       <c r="D187" t="s"/>
       <c r="E187" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F187" t="s"/>
       <c r="G187" t="s"/>
@@ -7698,15 +7695,15 @@
     </row>
     <row r="188" spans="1:14">
       <c r="A188" t="s">
+        <v>641</v>
+      </c>
+      <c r="B188" t="s">
         <v>642</v>
-      </c>
-      <c r="B188" t="s">
-        <v>643</v>
       </c>
       <c r="C188" t="s"/>
       <c r="D188" t="s"/>
       <c r="E188" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F188" t="s"/>
       <c r="G188" t="s"/>
@@ -7720,15 +7717,15 @@
     </row>
     <row r="189" spans="1:14">
       <c r="A189" t="s">
+        <v>644</v>
+      </c>
+      <c r="B189" t="s">
         <v>645</v>
-      </c>
-      <c r="B189" t="s">
-        <v>646</v>
       </c>
       <c r="C189" t="s"/>
       <c r="D189" t="s"/>
       <c r="E189" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F189" t="s"/>
       <c r="G189" t="s"/>
@@ -7742,15 +7739,15 @@
     </row>
     <row r="190" spans="1:14">
       <c r="A190" t="s">
+        <v>647</v>
+      </c>
+      <c r="B190" t="s">
         <v>648</v>
-      </c>
-      <c r="B190" t="s">
-        <v>649</v>
       </c>
       <c r="C190" t="s"/>
       <c r="D190" t="s"/>
       <c r="E190" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F190" t="s"/>
       <c r="G190" t="s"/>
@@ -7764,15 +7761,15 @@
     </row>
     <row r="191" spans="1:14">
       <c r="A191" t="s">
+        <v>650</v>
+      </c>
+      <c r="B191" t="s">
         <v>651</v>
-      </c>
-      <c r="B191" t="s">
-        <v>652</v>
       </c>
       <c r="C191" t="s"/>
       <c r="D191" t="s"/>
       <c r="E191" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F191" t="s"/>
       <c r="G191" t="s"/>
@@ -7786,7 +7783,7 @@
     </row>
     <row r="192" spans="1:14">
       <c r="A192" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B192" t="s">
         <v>123</v>
@@ -7794,7 +7791,7 @@
       <c r="C192" t="s"/>
       <c r="D192" t="s"/>
       <c r="E192" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F192" t="s"/>
       <c r="G192" t="s"/>
@@ -7808,15 +7805,15 @@
     </row>
     <row r="193" spans="1:14">
       <c r="A193" t="s">
+        <v>655</v>
+      </c>
+      <c r="B193" t="s">
         <v>656</v>
-      </c>
-      <c r="B193" t="s">
-        <v>657</v>
       </c>
       <c r="C193" t="s"/>
       <c r="D193" t="s"/>
       <c r="E193" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F193" t="s"/>
       <c r="G193" t="s"/>
@@ -7830,15 +7827,15 @@
     </row>
     <row r="194" spans="1:14">
       <c r="A194" t="s">
+        <v>658</v>
+      </c>
+      <c r="B194" t="s">
         <v>659</v>
-      </c>
-      <c r="B194" t="s">
-        <v>660</v>
       </c>
       <c r="C194" t="s"/>
       <c r="D194" t="s"/>
       <c r="E194" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F194" t="s"/>
       <c r="G194" t="s"/>
@@ -7852,15 +7849,15 @@
     </row>
     <row r="195" spans="1:14">
       <c r="A195" t="s">
+        <v>661</v>
+      </c>
+      <c r="B195" t="s">
         <v>662</v>
-      </c>
-      <c r="B195" t="s">
-        <v>663</v>
       </c>
       <c r="C195" t="s"/>
       <c r="D195" t="s"/>
       <c r="E195" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F195" t="s"/>
       <c r="G195" t="s"/>
@@ -7874,15 +7871,15 @@
     </row>
     <row r="196" spans="1:14">
       <c r="A196" t="s">
+        <v>664</v>
+      </c>
+      <c r="B196" t="s">
         <v>665</v>
-      </c>
-      <c r="B196" t="s">
-        <v>666</v>
       </c>
       <c r="C196" t="s"/>
       <c r="D196" t="s"/>
       <c r="E196" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F196" t="s"/>
       <c r="G196" t="s"/>
@@ -7896,15 +7893,15 @@
     </row>
     <row r="197" spans="1:14">
       <c r="A197" t="s">
+        <v>667</v>
+      </c>
+      <c r="B197" t="s">
         <v>668</v>
-      </c>
-      <c r="B197" t="s">
-        <v>669</v>
       </c>
       <c r="C197" t="s"/>
       <c r="D197" t="s"/>
       <c r="E197" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F197" t="s"/>
       <c r="G197" t="s"/>
@@ -7918,15 +7915,15 @@
     </row>
     <row r="198" spans="1:14">
       <c r="A198" t="s">
+        <v>670</v>
+      </c>
+      <c r="B198" t="s">
         <v>671</v>
-      </c>
-      <c r="B198" t="s">
-        <v>672</v>
       </c>
       <c r="C198" t="s"/>
       <c r="D198" t="s"/>
       <c r="E198" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="F198" t="s"/>
       <c r="G198" t="s"/>
@@ -7940,15 +7937,15 @@
     </row>
     <row r="199" spans="1:14">
       <c r="A199" t="s">
+        <v>673</v>
+      </c>
+      <c r="B199" t="s">
         <v>674</v>
-      </c>
-      <c r="B199" t="s">
-        <v>675</v>
       </c>
       <c r="C199" t="s"/>
       <c r="D199" t="s"/>
       <c r="E199" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F199" t="s"/>
       <c r="G199" t="s"/>
@@ -7962,15 +7959,15 @@
     </row>
     <row r="200" spans="1:14">
       <c r="A200" t="s">
+        <v>676</v>
+      </c>
+      <c r="B200" t="s">
         <v>677</v>
-      </c>
-      <c r="B200" t="s">
-        <v>678</v>
       </c>
       <c r="C200" t="s"/>
       <c r="D200" t="s"/>
       <c r="E200" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F200" t="s"/>
       <c r="G200" t="s"/>
@@ -7984,15 +7981,15 @@
     </row>
     <row r="201" spans="1:14">
       <c r="A201" t="s">
+        <v>679</v>
+      </c>
+      <c r="B201" t="s">
         <v>680</v>
-      </c>
-      <c r="B201" t="s">
-        <v>681</v>
       </c>
       <c r="C201" t="s"/>
       <c r="D201" t="s"/>
       <c r="E201" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F201" t="s"/>
       <c r="G201" t="s"/>
@@ -8006,15 +8003,15 @@
     </row>
     <row r="202" spans="1:14">
       <c r="A202" t="s">
+        <v>682</v>
+      </c>
+      <c r="B202" t="s">
         <v>683</v>
-      </c>
-      <c r="B202" t="s">
-        <v>684</v>
       </c>
       <c r="C202" t="s"/>
       <c r="D202" t="s"/>
       <c r="E202" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F202" t="s"/>
       <c r="G202" t="s"/>
@@ -8028,15 +8025,15 @@
     </row>
     <row r="203" spans="1:14">
       <c r="A203" t="s">
+        <v>685</v>
+      </c>
+      <c r="B203" t="s">
         <v>686</v>
-      </c>
-      <c r="B203" t="s">
-        <v>687</v>
       </c>
       <c r="C203" t="s"/>
       <c r="D203" t="s"/>
       <c r="E203" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F203" t="s"/>
       <c r="G203" t="s"/>
@@ -8050,7 +8047,7 @@
     </row>
     <row r="204" spans="1:14">
       <c r="A204" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B204" t="s">
         <v>163</v>
@@ -8058,7 +8055,7 @@
       <c r="C204" t="s"/>
       <c r="D204" t="s"/>
       <c r="E204" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F204" t="s"/>
       <c r="G204" t="s"/>
@@ -8072,15 +8069,15 @@
     </row>
     <row r="205" spans="1:14">
       <c r="A205" t="s">
+        <v>689</v>
+      </c>
+      <c r="B205" t="s">
         <v>690</v>
-      </c>
-      <c r="B205" t="s">
-        <v>691</v>
       </c>
       <c r="C205" t="s"/>
       <c r="D205" t="s"/>
       <c r="E205" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F205" t="s"/>
       <c r="G205" t="s"/>
@@ -8094,15 +8091,15 @@
     </row>
     <row r="206" spans="1:14">
       <c r="A206" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B206" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C206" t="s"/>
       <c r="D206" t="s"/>
       <c r="E206" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F206" t="s"/>
       <c r="G206" t="s"/>
@@ -8116,15 +8113,15 @@
     </row>
     <row r="207" spans="1:14">
       <c r="A207" t="s">
+        <v>694</v>
+      </c>
+      <c r="B207" t="s">
         <v>695</v>
-      </c>
-      <c r="B207" t="s">
-        <v>696</v>
       </c>
       <c r="C207" t="s"/>
       <c r="D207" t="s"/>
       <c r="E207" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="F207" t="s"/>
       <c r="G207" t="s"/>
@@ -8138,15 +8135,15 @@
     </row>
     <row r="208" spans="1:14">
       <c r="A208" t="s">
+        <v>696</v>
+      </c>
+      <c r="B208" t="s">
         <v>697</v>
-      </c>
-      <c r="B208" t="s">
-        <v>698</v>
       </c>
       <c r="C208" t="s"/>
       <c r="D208" t="s"/>
       <c r="E208" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F208" t="s"/>
       <c r="G208" t="s"/>
@@ -8160,15 +8157,15 @@
     </row>
     <row r="209" spans="1:14">
       <c r="A209" t="s">
+        <v>699</v>
+      </c>
+      <c r="B209" t="s">
         <v>700</v>
-      </c>
-      <c r="B209" t="s">
-        <v>701</v>
       </c>
       <c r="C209" t="s"/>
       <c r="D209" t="s"/>
       <c r="E209" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F209" t="s"/>
       <c r="G209" t="s"/>
@@ -8182,15 +8179,15 @@
     </row>
     <row r="210" spans="1:14">
       <c r="A210" t="s">
+        <v>702</v>
+      </c>
+      <c r="B210" t="s">
         <v>703</v>
-      </c>
-      <c r="B210" t="s">
-        <v>704</v>
       </c>
       <c r="C210" t="s"/>
       <c r="D210" t="s"/>
       <c r="E210" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F210" t="s"/>
       <c r="G210" t="s"/>
@@ -8204,15 +8201,15 @@
     </row>
     <row r="211" spans="1:14">
       <c r="A211" t="s">
+        <v>705</v>
+      </c>
+      <c r="B211" t="s">
         <v>706</v>
-      </c>
-      <c r="B211" t="s">
-        <v>707</v>
       </c>
       <c r="C211" t="s"/>
       <c r="D211" t="s"/>
       <c r="E211" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F211" t="s"/>
       <c r="G211" t="s"/>
@@ -8226,15 +8223,15 @@
     </row>
     <row r="212" spans="1:14">
       <c r="A212" t="s">
+        <v>708</v>
+      </c>
+      <c r="B212" t="s">
         <v>709</v>
-      </c>
-      <c r="B212" t="s">
-        <v>710</v>
       </c>
       <c r="C212" t="s"/>
       <c r="D212" t="s"/>
       <c r="E212" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F212" t="s"/>
       <c r="G212" t="s"/>
@@ -8248,15 +8245,15 @@
     </row>
     <row r="213" spans="1:14">
       <c r="A213" t="s">
+        <v>711</v>
+      </c>
+      <c r="B213" t="s">
         <v>712</v>
-      </c>
-      <c r="B213" t="s">
-        <v>713</v>
       </c>
       <c r="C213" t="s"/>
       <c r="D213" t="s"/>
       <c r="E213" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F213" t="s"/>
       <c r="G213" t="s"/>
@@ -8270,13 +8267,13 @@
     </row>
     <row r="214" spans="1:14">
       <c r="A214" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B214" t="s"/>
       <c r="C214" t="s"/>
       <c r="D214" t="s"/>
       <c r="E214" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F214" t="s"/>
       <c r="G214" t="s"/>
@@ -8290,13 +8287,13 @@
     </row>
     <row r="215" spans="1:14">
       <c r="A215" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B215" t="s"/>
       <c r="C215" t="s"/>
       <c r="D215" t="s"/>
       <c r="E215" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F215" t="s"/>
       <c r="G215" t="s"/>
@@ -8310,13 +8307,13 @@
     </row>
     <row r="216" spans="1:14">
       <c r="A216" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B216" t="s"/>
       <c r="C216" t="s"/>
       <c r="D216" t="s"/>
       <c r="E216" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F216" t="s"/>
       <c r="G216" t="s"/>
@@ -8330,13 +8327,13 @@
     </row>
     <row r="217" spans="1:14">
       <c r="A217" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B217" t="s"/>
       <c r="C217" t="s"/>
       <c r="D217" t="s"/>
       <c r="E217" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F217" t="s"/>
       <c r="G217" t="s"/>
@@ -8350,13 +8347,13 @@
     </row>
     <row r="218" spans="1:14">
       <c r="A218" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B218" t="s"/>
       <c r="C218" t="s"/>
       <c r="D218" t="s"/>
       <c r="E218" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F218" t="s"/>
       <c r="G218" t="s"/>
@@ -8370,7 +8367,7 @@
     </row>
     <row r="219" spans="1:14">
       <c r="A219" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B219" t="s"/>
       <c r="C219" t="s"/>
@@ -8390,13 +8387,13 @@
     </row>
     <row r="220" spans="1:14">
       <c r="A220" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B220" t="s"/>
       <c r="C220" t="s"/>
       <c r="D220" t="s"/>
       <c r="E220" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F220" t="s"/>
       <c r="G220" t="s"/>
@@ -8410,7 +8407,7 @@
     </row>
     <row r="221" spans="1:14">
       <c r="A221" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B221" t="s"/>
       <c r="C221" t="s"/>
@@ -8436,7 +8433,7 @@
       <c r="C222" t="s"/>
       <c r="D222" t="s"/>
       <c r="E222" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F222" t="s"/>
       <c r="G222" t="s"/>
@@ -8450,13 +8447,13 @@
     </row>
     <row r="223" spans="1:14">
       <c r="A223" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B223" t="s"/>
       <c r="C223" t="s"/>
       <c r="D223" t="s"/>
       <c r="E223" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F223" t="s"/>
       <c r="G223" t="s"/>
@@ -8470,13 +8467,13 @@
     </row>
     <row r="224" spans="1:14">
       <c r="A224" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B224" t="s"/>
       <c r="C224" t="s"/>
       <c r="D224" t="s"/>
       <c r="E224" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F224" t="s"/>
       <c r="G224" t="s"/>
@@ -8490,13 +8487,13 @@
     </row>
     <row r="225" spans="1:14">
       <c r="A225" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B225" t="s"/>
       <c r="C225" t="s"/>
       <c r="D225" t="s"/>
       <c r="E225" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F225" t="s"/>
       <c r="G225" t="s"/>
@@ -8510,13 +8507,13 @@
     </row>
     <row r="226" spans="1:14">
       <c r="A226" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B226" t="s"/>
       <c r="C226" t="s"/>
       <c r="D226" t="s"/>
       <c r="E226" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F226" t="s"/>
       <c r="G226" t="s"/>
@@ -8530,13 +8527,13 @@
     </row>
     <row r="227" spans="1:14">
       <c r="A227" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B227" t="s"/>
       <c r="C227" t="s"/>
       <c r="D227" t="s"/>
       <c r="E227" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F227" t="s"/>
       <c r="G227" t="s"/>
@@ -8550,13 +8547,13 @@
     </row>
     <row r="228" spans="1:14">
       <c r="A228" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B228" t="s"/>
       <c r="C228" t="s"/>
       <c r="D228" t="s"/>
       <c r="E228" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F228" t="s"/>
       <c r="G228" t="s"/>
@@ -8570,13 +8567,13 @@
     </row>
     <row r="229" spans="1:14">
       <c r="A229" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B229" t="s"/>
       <c r="C229" t="s"/>
       <c r="D229" t="s"/>
       <c r="E229" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F229" t="s"/>
       <c r="G229" t="s"/>
@@ -8590,13 +8587,13 @@
     </row>
     <row r="230" spans="1:14">
       <c r="A230" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B230" t="s"/>
       <c r="C230" t="s"/>
       <c r="D230" t="s"/>
       <c r="E230" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F230" t="s"/>
       <c r="G230" t="s"/>
@@ -8610,13 +8607,13 @@
     </row>
     <row r="231" spans="1:14">
       <c r="A231" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B231" t="s"/>
       <c r="C231" t="s"/>
       <c r="D231" t="s"/>
       <c r="E231" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F231" t="s"/>
       <c r="G231" t="s"/>
@@ -8630,13 +8627,13 @@
     </row>
     <row r="232" spans="1:14">
       <c r="A232" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B232" t="s"/>
       <c r="C232" t="s"/>
       <c r="D232" t="s"/>
       <c r="E232" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F232" t="s"/>
       <c r="G232" t="s"/>
@@ -8650,13 +8647,13 @@
     </row>
     <row r="233" spans="1:14">
       <c r="A233" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B233" t="s"/>
       <c r="C233" t="s"/>
       <c r="D233" t="s"/>
       <c r="E233" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F233" t="s"/>
       <c r="G233" t="s"/>
@@ -8670,13 +8667,13 @@
     </row>
     <row r="234" spans="1:14">
       <c r="A234" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B234" t="s"/>
       <c r="C234" t="s"/>
       <c r="D234" t="s"/>
       <c r="E234" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F234" t="s"/>
       <c r="G234" t="s"/>
@@ -8690,13 +8687,13 @@
     </row>
     <row r="235" spans="1:14">
       <c r="A235" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B235" t="s"/>
       <c r="C235" t="s"/>
       <c r="D235" t="s"/>
       <c r="E235" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F235" t="s"/>
       <c r="G235" t="s"/>
@@ -8710,13 +8707,13 @@
     </row>
     <row r="236" spans="1:14">
       <c r="A236" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B236" t="s"/>
       <c r="C236" t="s"/>
       <c r="D236" t="s"/>
       <c r="E236" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F236" t="s"/>
       <c r="G236" t="s"/>
@@ -8730,13 +8727,13 @@
     </row>
     <row r="237" spans="1:14">
       <c r="A237" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B237" t="s"/>
       <c r="C237" t="s"/>
       <c r="D237" t="s"/>
       <c r="E237" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F237" t="s"/>
       <c r="G237" t="s"/>
@@ -8750,13 +8747,13 @@
     </row>
     <row r="238" spans="1:14">
       <c r="A238" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B238" t="s"/>
       <c r="C238" t="s"/>
       <c r="D238" t="s"/>
       <c r="E238" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F238" t="s"/>
       <c r="G238" t="s"/>
@@ -8770,13 +8767,13 @@
     </row>
     <row r="239" spans="1:14">
       <c r="A239" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B239" t="s"/>
       <c r="C239" t="s"/>
       <c r="D239" t="s"/>
       <c r="E239" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F239" t="s"/>
       <c r="G239" t="s"/>
@@ -8790,13 +8787,13 @@
     </row>
     <row r="240" spans="1:14">
       <c r="A240" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B240" t="s"/>
       <c r="C240" t="s"/>
       <c r="D240" t="s"/>
       <c r="E240" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F240" t="s"/>
       <c r="G240" t="s"/>
@@ -8810,13 +8807,13 @@
     </row>
     <row r="241" spans="1:14">
       <c r="A241" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B241" t="s"/>
       <c r="C241" t="s"/>
       <c r="D241" t="s"/>
       <c r="E241" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F241" t="s"/>
       <c r="G241" t="s"/>
@@ -8830,13 +8827,13 @@
     </row>
     <row r="242" spans="1:14">
       <c r="A242" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B242" t="s"/>
       <c r="C242" t="s"/>
       <c r="D242" t="s"/>
       <c r="E242" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F242" t="s"/>
       <c r="G242" t="s"/>
@@ -8850,13 +8847,13 @@
     </row>
     <row r="243" spans="1:14">
       <c r="A243" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B243" t="s"/>
       <c r="C243" t="s"/>
       <c r="D243" t="s"/>
       <c r="E243" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F243" t="s"/>
       <c r="G243" t="s"/>
@@ -8870,13 +8867,13 @@
     </row>
     <row r="244" spans="1:14">
       <c r="A244" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B244" t="s"/>
       <c r="C244" t="s"/>
       <c r="D244" t="s"/>
       <c r="E244" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F244" t="s"/>
       <c r="G244" t="s"/>
@@ -8890,13 +8887,13 @@
     </row>
     <row r="245" spans="1:14">
       <c r="A245" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B245" t="s"/>
       <c r="C245" t="s"/>
       <c r="D245" t="s"/>
       <c r="E245" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F245" t="s"/>
       <c r="G245" t="s"/>
@@ -8910,13 +8907,13 @@
     </row>
     <row r="246" spans="1:14">
       <c r="A246" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B246" t="s"/>
       <c r="C246" t="s"/>
       <c r="D246" t="s"/>
       <c r="E246" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F246" t="s"/>
       <c r="G246" t="s"/>
@@ -8930,13 +8927,13 @@
     </row>
     <row r="247" spans="1:14">
       <c r="A247" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B247" t="s"/>
       <c r="C247" t="s"/>
       <c r="D247" t="s"/>
       <c r="E247" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F247" t="s"/>
       <c r="G247" t="s"/>
@@ -8950,13 +8947,13 @@
     </row>
     <row r="248" spans="1:14">
       <c r="A248" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B248" t="s"/>
       <c r="C248" t="s"/>
       <c r="D248" t="s"/>
       <c r="E248" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F248" t="s"/>
       <c r="G248" t="s"/>
@@ -8970,13 +8967,13 @@
     </row>
     <row r="249" spans="1:14">
       <c r="A249" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B249" t="s"/>
       <c r="C249" t="s"/>
       <c r="D249" t="s"/>
       <c r="E249" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F249" t="s"/>
       <c r="G249" t="s"/>
@@ -8990,13 +8987,13 @@
     </row>
     <row r="250" spans="1:14">
       <c r="A250" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B250" t="s"/>
       <c r="C250" t="s"/>
       <c r="D250" t="s"/>
       <c r="E250" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F250" t="s"/>
       <c r="G250" t="s"/>
@@ -9010,13 +9007,13 @@
     </row>
     <row r="251" spans="1:14">
       <c r="A251" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B251" t="s"/>
       <c r="C251" t="s"/>
       <c r="D251" t="s"/>
       <c r="E251" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F251" t="s"/>
       <c r="G251" t="s"/>
@@ -9030,7 +9027,7 @@
     </row>
     <row r="252" spans="1:14">
       <c r="A252" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B252" t="s"/>
       <c r="C252" t="s"/>
@@ -9048,7 +9045,7 @@
     </row>
     <row r="253" spans="1:14">
       <c r="A253" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B253" t="s"/>
       <c r="C253" t="s"/>
@@ -9066,7 +9063,7 @@
     </row>
     <row r="254" spans="1:14">
       <c r="A254" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B254" t="s"/>
       <c r="C254" t="s"/>
@@ -9084,7 +9081,7 @@
     </row>
     <row r="255" spans="1:14">
       <c r="A255" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B255" t="s"/>
       <c r="C255" t="s"/>
@@ -9102,7 +9099,7 @@
     </row>
     <row r="256" spans="1:14">
       <c r="A256" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B256" t="s"/>
       <c r="C256" t="s"/>
@@ -9120,7 +9117,7 @@
     </row>
     <row r="257" spans="1:14">
       <c r="A257" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B257" t="s"/>
       <c r="C257" t="s"/>
@@ -9138,7 +9135,7 @@
     </row>
     <row r="258" spans="1:14">
       <c r="A258" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B258" t="s"/>
       <c r="C258" t="s"/>
@@ -9156,7 +9153,7 @@
     </row>
     <row r="259" spans="1:14">
       <c r="A259" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B259" t="s"/>
       <c r="C259" t="s"/>
@@ -9174,7 +9171,7 @@
     </row>
     <row r="260" spans="1:14">
       <c r="A260" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B260" t="s"/>
       <c r="C260" t="s"/>
@@ -9192,7 +9189,7 @@
     </row>
     <row r="261" spans="1:14">
       <c r="A261" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B261" t="s"/>
       <c r="C261" t="s"/>
@@ -9210,7 +9207,7 @@
     </row>
     <row r="262" spans="1:14">
       <c r="A262" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B262" t="s"/>
       <c r="C262" t="s"/>
@@ -9228,7 +9225,7 @@
     </row>
     <row r="263" spans="1:14">
       <c r="A263" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B263" t="s"/>
       <c r="C263" t="s"/>
@@ -9246,7 +9243,7 @@
     </row>
     <row r="264" spans="1:14">
       <c r="A264" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B264" t="s"/>
       <c r="C264" t="s"/>
@@ -9264,7 +9261,7 @@
     </row>
     <row r="265" spans="1:14">
       <c r="A265" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B265" t="s"/>
       <c r="C265" t="s"/>
@@ -9282,7 +9279,7 @@
     </row>
     <row r="266" spans="1:14">
       <c r="A266" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B266" t="s"/>
       <c r="C266" t="s"/>
@@ -9300,7 +9297,7 @@
     </row>
     <row r="267" spans="1:14">
       <c r="A267" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B267" t="s"/>
       <c r="C267" t="s"/>
@@ -9318,7 +9315,7 @@
     </row>
     <row r="268" spans="1:14">
       <c r="A268" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="B268" t="s"/>
       <c r="C268" t="s"/>
@@ -9336,7 +9333,7 @@
     </row>
     <row r="269" spans="1:14">
       <c r="A269" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B269" t="s"/>
       <c r="C269" t="s"/>
@@ -9354,7 +9351,7 @@
     </row>
     <row r="270" spans="1:14">
       <c r="A270" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="B270" t="s"/>
       <c r="C270" t="s"/>
@@ -9372,7 +9369,7 @@
     </row>
     <row r="271" spans="1:14">
       <c r="A271" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B271" t="s"/>
       <c r="C271" t="s"/>
@@ -9390,7 +9387,7 @@
     </row>
     <row r="272" spans="1:14">
       <c r="A272" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B272" t="s"/>
       <c r="C272" t="s"/>
@@ -9408,7 +9405,7 @@
     </row>
     <row r="273" spans="1:14">
       <c r="A273" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B273" t="s"/>
       <c r="C273" t="s"/>
@@ -9426,7 +9423,7 @@
     </row>
     <row r="274" spans="1:14">
       <c r="A274" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B274" t="s"/>
       <c r="C274" t="s"/>
@@ -9444,7 +9441,7 @@
     </row>
     <row r="275" spans="1:14">
       <c r="A275" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B275" t="s"/>
       <c r="C275" t="s"/>
@@ -9462,7 +9459,7 @@
     </row>
     <row r="276" spans="1:14">
       <c r="A276" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B276" t="s"/>
       <c r="C276" t="s"/>
@@ -9480,7 +9477,7 @@
     </row>
     <row r="277" spans="1:14">
       <c r="A277" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B277" t="s"/>
       <c r="C277" t="s"/>
@@ -9498,7 +9495,7 @@
     </row>
     <row r="278" spans="1:14">
       <c r="A278" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B278" t="s"/>
       <c r="C278" t="s"/>
@@ -9516,7 +9513,7 @@
     </row>
     <row r="279" spans="1:14">
       <c r="A279" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B279" t="s"/>
       <c r="C279" t="s"/>
@@ -9534,7 +9531,7 @@
     </row>
     <row r="280" spans="1:14">
       <c r="A280" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B280" t="s"/>
       <c r="C280" t="s"/>
@@ -9552,7 +9549,7 @@
     </row>
     <row r="281" spans="1:14">
       <c r="A281" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B281" t="s"/>
       <c r="C281" t="s"/>
@@ -9570,7 +9567,7 @@
     </row>
     <row r="282" spans="1:14">
       <c r="A282" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B282" t="s"/>
       <c r="C282" t="s"/>
@@ -9588,7 +9585,7 @@
     </row>
     <row r="283" spans="1:14">
       <c r="A283" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B283" t="s"/>
       <c r="C283" t="s"/>
@@ -9606,7 +9603,7 @@
     </row>
     <row r="284" spans="1:14">
       <c r="A284" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B284" t="s"/>
       <c r="C284" t="s"/>
@@ -9624,7 +9621,7 @@
     </row>
     <row r="285" spans="1:14">
       <c r="A285" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B285" t="s"/>
       <c r="C285" t="s"/>
@@ -9642,7 +9639,7 @@
     </row>
     <row r="286" spans="1:14">
       <c r="A286" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B286" t="s"/>
       <c r="C286" t="s"/>
@@ -9660,7 +9657,7 @@
     </row>
     <row r="287" spans="1:14">
       <c r="A287" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B287" t="s"/>
       <c r="C287" t="s"/>
@@ -9678,7 +9675,7 @@
     </row>
     <row r="288" spans="1:14">
       <c r="A288" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B288" t="s"/>
       <c r="C288" t="s"/>
@@ -9696,7 +9693,7 @@
     </row>
     <row r="289" spans="1:14">
       <c r="A289" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B289" t="s"/>
       <c r="C289" t="s"/>
@@ -9714,7 +9711,7 @@
     </row>
     <row r="290" spans="1:14">
       <c r="A290" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B290" t="s"/>
       <c r="C290" t="s"/>
@@ -9732,7 +9729,7 @@
     </row>
     <row r="291" spans="1:14">
       <c r="A291" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B291" t="s"/>
       <c r="C291" t="s"/>
@@ -9750,7 +9747,7 @@
     </row>
     <row r="292" spans="1:14">
       <c r="A292" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B292" t="s"/>
       <c r="C292" t="s"/>
@@ -9768,7 +9765,7 @@
     </row>
     <row r="293" spans="1:14">
       <c r="A293" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B293" t="s"/>
       <c r="C293" t="s"/>
@@ -9786,7 +9783,7 @@
     </row>
     <row r="294" spans="1:14">
       <c r="A294" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B294" t="s"/>
       <c r="C294" t="s"/>
@@ -9804,7 +9801,7 @@
     </row>
     <row r="295" spans="1:14">
       <c r="A295" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B295" t="s"/>
       <c r="C295" t="s"/>
@@ -9822,7 +9819,7 @@
     </row>
     <row r="296" spans="1:14">
       <c r="A296" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B296" t="s"/>
       <c r="C296" t="s"/>
@@ -9840,7 +9837,7 @@
     </row>
     <row r="297" spans="1:14">
       <c r="A297" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B297" t="s"/>
       <c r="C297" t="s"/>
@@ -9858,7 +9855,7 @@
     </row>
     <row r="298" spans="1:14">
       <c r="A298" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B298" t="s"/>
       <c r="C298" t="s"/>
@@ -10146,7 +10143,7 @@
     </row>
     <row r="314" spans="1:14">
       <c r="A314" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B314" t="s"/>
       <c r="C314" t="s"/>
@@ -10164,7 +10161,7 @@
     </row>
     <row r="315" spans="1:14">
       <c r="A315" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B315" t="s"/>
       <c r="C315" t="s"/>
@@ -10182,7 +10179,7 @@
     </row>
     <row r="316" spans="1:14">
       <c r="A316" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B316" t="s"/>
       <c r="C316" t="s"/>
@@ -10200,7 +10197,7 @@
     </row>
     <row r="317" spans="1:14">
       <c r="A317" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B317" t="s"/>
       <c r="C317" t="s"/>
@@ -10218,7 +10215,7 @@
     </row>
     <row r="318" spans="1:14">
       <c r="A318" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B318" t="s"/>
       <c r="C318" t="s"/>
@@ -10236,7 +10233,7 @@
     </row>
     <row r="319" spans="1:14">
       <c r="A319" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B319" t="s"/>
       <c r="C319" t="s"/>
@@ -10254,7 +10251,7 @@
     </row>
     <row r="320" spans="1:14">
       <c r="A320" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B320" t="s"/>
       <c r="C320" t="s"/>
@@ -10272,7 +10269,7 @@
     </row>
     <row r="321" spans="1:14">
       <c r="A321" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B321" t="s"/>
       <c r="C321" t="s"/>
@@ -10290,7 +10287,7 @@
     </row>
     <row r="322" spans="1:14">
       <c r="A322" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B322" t="s"/>
       <c r="C322" t="s"/>
@@ -10308,7 +10305,7 @@
     </row>
     <row r="323" spans="1:14">
       <c r="A323" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B323" t="s"/>
       <c r="C323" t="s"/>
@@ -10326,7 +10323,7 @@
     </row>
     <row r="324" spans="1:14">
       <c r="A324" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B324" t="s"/>
       <c r="C324" t="s"/>
@@ -10362,7 +10359,7 @@
     </row>
     <row r="326" spans="1:14">
       <c r="A326" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B326" t="s"/>
       <c r="C326" t="s"/>
@@ -10380,7 +10377,7 @@
     </row>
     <row r="327" spans="1:14">
       <c r="A327" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="B327" t="s"/>
       <c r="C327" t="s"/>
@@ -10398,7 +10395,7 @@
     </row>
     <row r="328" spans="1:14">
       <c r="A328" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B328" t="s"/>
       <c r="C328" t="s"/>
@@ -10416,7 +10413,7 @@
     </row>
     <row r="329" spans="1:14">
       <c r="A329" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B329" t="s"/>
       <c r="C329" t="s"/>
@@ -10434,7 +10431,7 @@
     </row>
     <row r="330" spans="1:14">
       <c r="A330" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B330" t="s"/>
       <c r="C330" t="s"/>
@@ -10452,7 +10449,7 @@
     </row>
     <row r="331" spans="1:14">
       <c r="A331" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B331" t="s"/>
       <c r="C331" t="s"/>
@@ -10470,7 +10467,7 @@
     </row>
     <row r="332" spans="1:14">
       <c r="A332" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="B332" t="s"/>
       <c r="C332" t="s"/>
@@ -10488,7 +10485,7 @@
     </row>
     <row r="333" spans="1:14">
       <c r="A333" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B333" t="s"/>
       <c r="C333" t="s"/>
@@ -10506,7 +10503,7 @@
     </row>
     <row r="334" spans="1:14">
       <c r="A334" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B334" t="s"/>
       <c r="C334" t="s"/>
@@ -10524,7 +10521,7 @@
     </row>
     <row r="335" spans="1:14">
       <c r="A335" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B335" t="s"/>
       <c r="C335" t="s"/>
@@ -10542,7 +10539,7 @@
     </row>
     <row r="336" spans="1:14">
       <c r="A336" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B336" t="s"/>
       <c r="C336" t="s"/>
@@ -10560,7 +10557,7 @@
     </row>
     <row r="337" spans="1:14">
       <c r="A337" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B337" t="s"/>
       <c r="C337" t="s"/>
@@ -10578,7 +10575,7 @@
     </row>
     <row r="338" spans="1:14">
       <c r="A338" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B338" t="s"/>
       <c r="C338" t="s"/>
@@ -10614,7 +10611,7 @@
     </row>
     <row r="340" spans="1:14">
       <c r="A340" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B340" t="s"/>
       <c r="C340" t="s"/>
@@ -10632,7 +10629,7 @@
     </row>
     <row r="341" spans="1:14">
       <c r="A341" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B341" t="s"/>
       <c r="C341" t="s"/>
@@ -10650,7 +10647,7 @@
     </row>
     <row r="342" spans="1:14">
       <c r="A342" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B342" t="s"/>
       <c r="C342" t="s"/>
@@ -10668,7 +10665,7 @@
     </row>
     <row r="343" spans="1:14">
       <c r="A343" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B343" t="s"/>
       <c r="C343" t="s"/>
@@ -10686,7 +10683,7 @@
     </row>
     <row r="344" spans="1:14">
       <c r="A344" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B344" t="s"/>
       <c r="C344" t="s"/>
@@ -10704,7 +10701,7 @@
     </row>
     <row r="345" spans="1:14">
       <c r="A345" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B345" t="s"/>
       <c r="C345" t="s"/>
@@ -10722,7 +10719,7 @@
     </row>
     <row r="346" spans="1:14">
       <c r="A346" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B346" t="s"/>
       <c r="C346" t="s"/>
@@ -10740,7 +10737,7 @@
     </row>
     <row r="347" spans="1:14">
       <c r="A347" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B347" t="s"/>
       <c r="C347" t="s"/>
@@ -10758,7 +10755,7 @@
     </row>
     <row r="348" spans="1:14">
       <c r="A348" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B348" t="s"/>
       <c r="C348" t="s"/>
@@ -10776,7 +10773,7 @@
     </row>
     <row r="349" spans="1:14">
       <c r="A349" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B349" t="s"/>
       <c r="C349" t="s"/>
@@ -10794,7 +10791,7 @@
     </row>
     <row r="350" spans="1:14">
       <c r="A350" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B350" t="s"/>
       <c r="C350" t="s"/>
@@ -10812,7 +10809,7 @@
     </row>
     <row r="351" spans="1:14">
       <c r="A351" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B351" t="s"/>
       <c r="C351" t="s"/>
@@ -10830,7 +10827,7 @@
     </row>
     <row r="352" spans="1:14">
       <c r="A352" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B352" t="s"/>
       <c r="C352" t="s"/>
@@ -10848,7 +10845,7 @@
     </row>
     <row r="353" spans="1:14">
       <c r="A353" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B353" t="s"/>
       <c r="C353" t="s"/>
@@ -10866,7 +10863,7 @@
     </row>
     <row r="354" spans="1:14">
       <c r="A354" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B354" t="s"/>
       <c r="C354" t="s"/>
@@ -10884,7 +10881,7 @@
     </row>
     <row r="355" spans="1:14">
       <c r="A355" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B355" t="s"/>
       <c r="C355" t="s"/>
@@ -10902,7 +10899,7 @@
     </row>
     <row r="356" spans="1:14">
       <c r="A356" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B356" t="s"/>
       <c r="C356" t="s"/>
@@ -10920,7 +10917,7 @@
     </row>
     <row r="357" spans="1:14">
       <c r="A357" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B357" t="s"/>
       <c r="C357" t="s"/>
@@ -10938,7 +10935,7 @@
     </row>
     <row r="358" spans="1:14">
       <c r="A358" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B358" t="s"/>
       <c r="C358" t="s"/>
@@ -10956,7 +10953,7 @@
     </row>
     <row r="359" spans="1:14">
       <c r="A359" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B359" t="s"/>
       <c r="C359" t="s"/>
@@ -10974,7 +10971,7 @@
     </row>
     <row r="360" spans="1:14">
       <c r="A360" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B360" t="s"/>
       <c r="C360" t="s"/>
@@ -10992,7 +10989,7 @@
     </row>
     <row r="361" spans="1:14">
       <c r="A361" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B361" t="s"/>
       <c r="C361" t="s"/>
@@ -11010,7 +11007,7 @@
     </row>
     <row r="362" spans="1:14">
       <c r="A362" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B362" t="s"/>
       <c r="C362" t="s"/>
@@ -11028,7 +11025,7 @@
     </row>
     <row r="363" spans="1:14">
       <c r="A363" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B363" t="s"/>
       <c r="C363" t="s"/>
@@ -11046,7 +11043,7 @@
     </row>
     <row r="364" spans="1:14">
       <c r="A364" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B364" t="s"/>
       <c r="C364" t="s"/>
@@ -11064,7 +11061,7 @@
     </row>
     <row r="365" spans="1:14">
       <c r="A365" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B365" t="s"/>
       <c r="C365" t="s"/>
@@ -11082,7 +11079,7 @@
     </row>
     <row r="366" spans="1:14">
       <c r="A366" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B366" t="s"/>
       <c r="C366" t="s"/>
@@ -11100,7 +11097,7 @@
     </row>
     <row r="367" spans="1:14">
       <c r="A367" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B367" t="s"/>
       <c r="C367" t="s"/>
@@ -11118,7 +11115,7 @@
     </row>
     <row r="368" spans="1:14">
       <c r="A368" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B368" t="s"/>
       <c r="C368" t="s"/>
@@ -11136,7 +11133,7 @@
     </row>
     <row r="369" spans="1:14">
       <c r="A369" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B369" t="s"/>
       <c r="C369" t="s"/>
@@ -11154,7 +11151,7 @@
     </row>
     <row r="370" spans="1:14">
       <c r="A370" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B370" t="s"/>
       <c r="C370" t="s"/>
@@ -11172,7 +11169,7 @@
     </row>
     <row r="371" spans="1:14">
       <c r="A371" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B371" t="s"/>
       <c r="C371" t="s"/>
@@ -11190,7 +11187,7 @@
     </row>
     <row r="372" spans="1:14">
       <c r="A372" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B372" t="s"/>
       <c r="C372" t="s"/>
@@ -11208,7 +11205,7 @@
     </row>
     <row r="373" spans="1:14">
       <c r="A373" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B373" t="s"/>
       <c r="C373" t="s"/>
@@ -11226,7 +11223,7 @@
     </row>
     <row r="374" spans="1:14">
       <c r="A374" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B374" t="s"/>
       <c r="C374" t="s"/>
@@ -11244,7 +11241,7 @@
     </row>
     <row r="375" spans="1:14">
       <c r="A375" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B375" t="s"/>
       <c r="C375" t="s"/>
@@ -11262,7 +11259,7 @@
     </row>
     <row r="376" spans="1:14">
       <c r="A376" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B376" t="s"/>
       <c r="C376" t="s"/>
@@ -11280,7 +11277,7 @@
     </row>
     <row r="377" spans="1:14">
       <c r="A377" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B377" t="s"/>
       <c r="C377" t="s"/>
@@ -11298,7 +11295,7 @@
     </row>
     <row r="378" spans="1:14">
       <c r="A378" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B378" t="s"/>
       <c r="C378" t="s"/>
@@ -11316,7 +11313,7 @@
     </row>
     <row r="379" spans="1:14">
       <c r="A379" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B379" t="s"/>
       <c r="C379" t="s"/>
@@ -11334,7 +11331,7 @@
     </row>
     <row r="380" spans="1:14">
       <c r="A380" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B380" t="s"/>
       <c r="C380" t="s"/>
@@ -11352,7 +11349,7 @@
     </row>
     <row r="381" spans="1:14">
       <c r="A381" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B381" t="s"/>
       <c r="C381" t="s"/>
@@ -11370,7 +11367,7 @@
     </row>
     <row r="382" spans="1:14">
       <c r="A382" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B382" t="s"/>
       <c r="C382" t="s"/>
@@ -11388,7 +11385,7 @@
     </row>
     <row r="383" spans="1:14">
       <c r="A383" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B383" t="s"/>
       <c r="C383" t="s"/>
@@ -11406,7 +11403,7 @@
     </row>
     <row r="384" spans="1:14">
       <c r="A384" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B384" t="s"/>
       <c r="C384" t="s"/>
@@ -11424,7 +11421,7 @@
     </row>
     <row r="385" spans="1:14">
       <c r="A385" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B385" t="s"/>
       <c r="C385" t="s"/>
@@ -11442,7 +11439,7 @@
     </row>
     <row r="386" spans="1:14">
       <c r="A386" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B386" t="s"/>
       <c r="C386" t="s"/>
@@ -11460,7 +11457,7 @@
     </row>
     <row r="387" spans="1:14">
       <c r="A387" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B387" t="s"/>
       <c r="C387" t="s"/>
@@ -11478,7 +11475,7 @@
     </row>
     <row r="388" spans="1:14">
       <c r="A388" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B388" t="s"/>
       <c r="C388" t="s"/>
@@ -11496,7 +11493,7 @@
     </row>
     <row r="389" spans="1:14">
       <c r="A389" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B389" t="s"/>
       <c r="C389" t="s"/>
@@ -11514,7 +11511,7 @@
     </row>
     <row r="390" spans="1:14">
       <c r="A390" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B390" t="s"/>
       <c r="C390" t="s"/>
@@ -11532,7 +11529,7 @@
     </row>
     <row r="391" spans="1:14">
       <c r="A391" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B391" t="s"/>
       <c r="C391" t="s"/>
@@ -11550,7 +11547,7 @@
     </row>
     <row r="392" spans="1:14">
       <c r="A392" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B392" t="s"/>
       <c r="C392" t="s"/>
@@ -11568,7 +11565,7 @@
     </row>
     <row r="393" spans="1:14">
       <c r="A393" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B393" t="s"/>
       <c r="C393" t="s"/>
@@ -11586,7 +11583,7 @@
     </row>
     <row r="394" spans="1:14">
       <c r="A394" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B394" t="s"/>
       <c r="C394" t="s"/>
@@ -11604,7 +11601,7 @@
     </row>
     <row r="395" spans="1:14">
       <c r="A395" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B395" t="s"/>
       <c r="C395" t="s"/>
@@ -11622,7 +11619,7 @@
     </row>
     <row r="396" spans="1:14">
       <c r="A396" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B396" t="s"/>
       <c r="C396" t="s"/>
@@ -11640,7 +11637,7 @@
     </row>
     <row r="397" spans="1:14">
       <c r="A397" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B397" t="s"/>
       <c r="C397" t="s"/>
@@ -11658,7 +11655,7 @@
     </row>
     <row r="398" spans="1:14">
       <c r="A398" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B398" t="s"/>
       <c r="C398" t="s"/>
@@ -11676,7 +11673,7 @@
     </row>
     <row r="399" spans="1:14">
       <c r="A399" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B399" t="s"/>
       <c r="C399" t="s"/>
@@ -11694,7 +11691,7 @@
     </row>
     <row r="400" spans="1:14">
       <c r="A400" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B400" t="s"/>
       <c r="C400" t="s"/>
@@ -11712,7 +11709,7 @@
     </row>
     <row r="401" spans="1:14">
       <c r="A401" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B401" t="s"/>
       <c r="C401" t="s"/>
@@ -11730,7 +11727,7 @@
     </row>
     <row r="402" spans="1:14">
       <c r="A402" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B402" t="s"/>
       <c r="C402" t="s"/>
@@ -11748,7 +11745,7 @@
     </row>
     <row r="403" spans="1:14">
       <c r="A403" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B403" t="s"/>
       <c r="C403" t="s"/>
@@ -11766,7 +11763,7 @@
     </row>
     <row r="404" spans="1:14">
       <c r="A404" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B404" t="s"/>
       <c r="C404" t="s"/>
@@ -11784,7 +11781,7 @@
     </row>
     <row r="405" spans="1:14">
       <c r="A405" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B405" t="s"/>
       <c r="C405" t="s"/>
@@ -11802,7 +11799,7 @@
     </row>
     <row r="406" spans="1:14">
       <c r="A406" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B406" t="s"/>
       <c r="C406" t="s"/>
@@ -11820,7 +11817,7 @@
     </row>
     <row r="407" spans="1:14">
       <c r="A407" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B407" t="s"/>
       <c r="C407" t="s"/>
@@ -11838,7 +11835,7 @@
     </row>
     <row r="408" spans="1:14">
       <c r="A408" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B408" t="s"/>
       <c r="C408" t="s"/>
@@ -11856,7 +11853,7 @@
     </row>
     <row r="409" spans="1:14">
       <c r="A409" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B409" t="s"/>
       <c r="C409" t="s"/>
@@ -11874,7 +11871,7 @@
     </row>
     <row r="410" spans="1:14">
       <c r="A410" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B410" t="s"/>
       <c r="C410" t="s"/>
@@ -11892,7 +11889,7 @@
     </row>
     <row r="411" spans="1:14">
       <c r="A411" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B411" t="s"/>
       <c r="C411" t="s"/>
@@ -11910,7 +11907,7 @@
     </row>
     <row r="412" spans="1:14">
       <c r="A412" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B412" t="s"/>
       <c r="C412" t="s"/>
@@ -11928,7 +11925,7 @@
     </row>
     <row r="413" spans="1:14">
       <c r="A413" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B413" t="s"/>
       <c r="C413" t="s"/>
@@ -11946,7 +11943,7 @@
     </row>
     <row r="414" spans="1:14">
       <c r="A414" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B414" t="s"/>
       <c r="C414" t="s"/>
@@ -11964,7 +11961,7 @@
     </row>
     <row r="415" spans="1:14">
       <c r="A415" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B415" t="s"/>
       <c r="C415" t="s"/>
@@ -11982,7 +11979,7 @@
     </row>
     <row r="416" spans="1:14">
       <c r="A416" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B416" t="s"/>
       <c r="C416" t="s"/>
@@ -12000,7 +11997,7 @@
     </row>
     <row r="417" spans="1:14">
       <c r="A417" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B417" t="s"/>
       <c r="C417" t="s"/>
@@ -12018,7 +12015,7 @@
     </row>
     <row r="418" spans="1:14">
       <c r="A418" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B418" t="s"/>
       <c r="C418" t="s"/>
@@ -12036,7 +12033,7 @@
     </row>
     <row r="419" spans="1:14">
       <c r="A419" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B419" t="s"/>
       <c r="C419" t="s"/>
@@ -12054,7 +12051,7 @@
     </row>
     <row r="420" spans="1:14">
       <c r="A420" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B420" t="s"/>
       <c r="C420" t="s"/>
@@ -12072,7 +12069,7 @@
     </row>
     <row r="421" spans="1:14">
       <c r="A421" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B421" t="s"/>
       <c r="C421" t="s"/>
@@ -12090,7 +12087,7 @@
     </row>
     <row r="422" spans="1:14">
       <c r="A422" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B422" t="s"/>
       <c r="C422" t="s"/>
@@ -12108,7 +12105,7 @@
     </row>
     <row r="423" spans="1:14">
       <c r="A423" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B423" t="s"/>
       <c r="C423" t="s"/>
@@ -12126,7 +12123,7 @@
     </row>
     <row r="424" spans="1:14">
       <c r="A424" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B424" t="s"/>
       <c r="C424" t="s"/>
@@ -12144,7 +12141,7 @@
     </row>
     <row r="425" spans="1:14">
       <c r="A425" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B425" t="s"/>
       <c r="C425" t="s"/>
@@ -12162,7 +12159,7 @@
     </row>
     <row r="426" spans="1:14">
       <c r="A426" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B426" t="s"/>
       <c r="C426" t="s"/>
@@ -12180,7 +12177,7 @@
     </row>
     <row r="427" spans="1:14">
       <c r="A427" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B427" t="s"/>
       <c r="C427" t="s"/>
@@ -12198,7 +12195,7 @@
     </row>
     <row r="428" spans="1:14">
       <c r="A428" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B428" t="s"/>
       <c r="C428" t="s"/>
@@ -12216,7 +12213,7 @@
     </row>
     <row r="429" spans="1:14">
       <c r="A429" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B429" t="s"/>
       <c r="C429" t="s"/>
@@ -12234,7 +12231,7 @@
     </row>
     <row r="430" spans="1:14">
       <c r="A430" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B430" t="s"/>
       <c r="C430" t="s"/>
@@ -12252,7 +12249,7 @@
     </row>
     <row r="431" spans="1:14">
       <c r="A431" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B431" t="s"/>
       <c r="C431" t="s"/>
@@ -12270,7 +12267,7 @@
     </row>
     <row r="432" spans="1:14">
       <c r="A432" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B432" t="s"/>
       <c r="C432" t="s"/>
@@ -12288,7 +12285,7 @@
     </row>
     <row r="433" spans="1:14">
       <c r="A433" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B433" t="s"/>
       <c r="C433" t="s"/>
@@ -12306,7 +12303,7 @@
     </row>
     <row r="434" spans="1:14">
       <c r="A434" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B434" t="s"/>
       <c r="C434" t="s"/>
@@ -12324,7 +12321,7 @@
     </row>
     <row r="435" spans="1:14">
       <c r="A435" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B435" t="s"/>
       <c r="C435" t="s"/>
@@ -12342,7 +12339,7 @@
     </row>
     <row r="436" spans="1:14">
       <c r="A436" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B436" t="s"/>
       <c r="C436" t="s"/>
@@ -12360,7 +12357,7 @@
     </row>
     <row r="437" spans="1:14">
       <c r="A437" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B437" t="s"/>
       <c r="C437" t="s"/>
@@ -12378,7 +12375,7 @@
     </row>
     <row r="438" spans="1:14">
       <c r="A438" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B438" t="s"/>
       <c r="C438" t="s"/>
@@ -12396,7 +12393,7 @@
     </row>
     <row r="439" spans="1:14">
       <c r="A439" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B439" t="s"/>
       <c r="C439" t="s"/>
@@ -12414,7 +12411,7 @@
     </row>
     <row r="440" spans="1:14">
       <c r="A440" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B440" t="s"/>
       <c r="C440" t="s"/>
@@ -12432,7 +12429,7 @@
     </row>
     <row r="441" spans="1:14">
       <c r="A441" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B441" t="s"/>
       <c r="C441" t="s"/>
@@ -12450,7 +12447,7 @@
     </row>
     <row r="442" spans="1:14">
       <c r="A442" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B442" t="s"/>
       <c r="C442" t="s"/>
@@ -12468,7 +12465,7 @@
     </row>
     <row r="443" spans="1:14">
       <c r="A443" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B443" t="s"/>
       <c r="C443" t="s"/>
@@ -12486,7 +12483,7 @@
     </row>
     <row r="444" spans="1:14">
       <c r="A444" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B444" t="s"/>
       <c r="C444" t="s"/>
@@ -12504,7 +12501,7 @@
     </row>
     <row r="445" spans="1:14">
       <c r="A445" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B445" t="s"/>
       <c r="C445" t="s"/>
@@ -12522,7 +12519,7 @@
     </row>
     <row r="446" spans="1:14">
       <c r="A446" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B446" t="s"/>
       <c r="C446" t="s"/>
@@ -12540,7 +12537,7 @@
     </row>
     <row r="447" spans="1:14">
       <c r="A447" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B447" t="s"/>
       <c r="C447" t="s"/>
@@ -12558,7 +12555,7 @@
     </row>
     <row r="448" spans="1:14">
       <c r="A448" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B448" t="s"/>
       <c r="C448" t="s"/>
@@ -12576,7 +12573,7 @@
     </row>
     <row r="449" spans="1:14">
       <c r="A449" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B449" t="s"/>
       <c r="C449" t="s"/>
@@ -12594,7 +12591,7 @@
     </row>
     <row r="450" spans="1:14">
       <c r="A450" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B450" t="s"/>
       <c r="C450" t="s"/>
@@ -12612,7 +12609,7 @@
     </row>
     <row r="451" spans="1:14">
       <c r="A451" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B451" t="s"/>
       <c r="C451" t="s"/>
@@ -12630,7 +12627,7 @@
     </row>
     <row r="452" spans="1:14">
       <c r="A452" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B452" t="s"/>
       <c r="C452" t="s"/>
@@ -12648,7 +12645,7 @@
     </row>
     <row r="453" spans="1:14">
       <c r="A453" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B453" t="s"/>
       <c r="C453" t="s"/>
@@ -12666,7 +12663,7 @@
     </row>
     <row r="454" spans="1:14">
       <c r="A454" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B454" t="s"/>
       <c r="C454" t="s"/>
@@ -12684,7 +12681,7 @@
     </row>
     <row r="455" spans="1:14">
       <c r="A455" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B455" t="s"/>
       <c r="C455" t="s"/>
@@ -12702,7 +12699,7 @@
     </row>
     <row r="456" spans="1:14">
       <c r="A456" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B456" t="s"/>
       <c r="C456" t="s"/>
@@ -12720,7 +12717,7 @@
     </row>
     <row r="457" spans="1:14">
       <c r="A457" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B457" t="s"/>
       <c r="C457" t="s"/>
@@ -12738,7 +12735,7 @@
     </row>
     <row r="458" spans="1:14">
       <c r="A458" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B458" t="s"/>
       <c r="C458" t="s"/>
@@ -12756,7 +12753,7 @@
     </row>
     <row r="459" spans="1:14">
       <c r="A459" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B459" t="s"/>
       <c r="C459" t="s"/>
@@ -12774,7 +12771,7 @@
     </row>
     <row r="460" spans="1:14">
       <c r="A460" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B460" t="s"/>
       <c r="C460" t="s"/>
@@ -12792,7 +12789,7 @@
     </row>
     <row r="461" spans="1:14">
       <c r="A461" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B461" t="s"/>
       <c r="C461" t="s"/>
@@ -12810,7 +12807,7 @@
     </row>
     <row r="462" spans="1:14">
       <c r="A462" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B462" t="s"/>
       <c r="C462" t="s"/>
@@ -12828,7 +12825,7 @@
     </row>
     <row r="463" spans="1:14">
       <c r="A463" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B463" t="s"/>
       <c r="C463" t="s"/>
@@ -12846,7 +12843,7 @@
     </row>
     <row r="464" spans="1:14">
       <c r="A464" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B464" t="s"/>
       <c r="C464" t="s"/>
@@ -12864,7 +12861,7 @@
     </row>
     <row r="465" spans="1:14">
       <c r="A465" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B465" t="s"/>
       <c r="C465" t="s"/>
@@ -12882,7 +12879,7 @@
     </row>
     <row r="466" spans="1:14">
       <c r="A466" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B466" t="s"/>
       <c r="C466" t="s"/>
@@ -12900,7 +12897,7 @@
     </row>
     <row r="467" spans="1:14">
       <c r="A467" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B467" t="s"/>
       <c r="C467" t="s"/>
@@ -12918,7 +12915,7 @@
     </row>
     <row r="468" spans="1:14">
       <c r="A468" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B468" t="s"/>
       <c r="C468" t="s"/>
@@ -12936,7 +12933,7 @@
     </row>
     <row r="469" spans="1:14">
       <c r="A469" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B469" t="s"/>
       <c r="C469" t="s"/>
@@ -12954,7 +12951,7 @@
     </row>
     <row r="470" spans="1:14">
       <c r="A470" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B470" t="s"/>
       <c r="C470" t="s"/>
@@ -12972,7 +12969,7 @@
     </row>
     <row r="471" spans="1:14">
       <c r="A471" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B471" t="s"/>
       <c r="C471" t="s"/>
@@ -12990,7 +12987,7 @@
     </row>
     <row r="472" spans="1:14">
       <c r="A472" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B472" t="s"/>
       <c r="C472" t="s"/>
@@ -13008,7 +13005,7 @@
     </row>
     <row r="473" spans="1:14">
       <c r="A473" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B473" t="s"/>
       <c r="C473" t="s"/>
@@ -13026,7 +13023,7 @@
     </row>
     <row r="474" spans="1:14">
       <c r="A474" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B474" t="s"/>
       <c r="C474" t="s"/>
@@ -13044,7 +13041,7 @@
     </row>
     <row r="475" spans="1:14">
       <c r="A475" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B475" t="s"/>
       <c r="C475" t="s"/>
@@ -13062,7 +13059,7 @@
     </row>
     <row r="476" spans="1:14">
       <c r="A476" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B476" t="s"/>
       <c r="C476" t="s"/>
@@ -13080,7 +13077,7 @@
     </row>
     <row r="477" spans="1:14">
       <c r="A477" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B477" t="s"/>
       <c r="C477" t="s"/>
@@ -13098,7 +13095,7 @@
     </row>
     <row r="478" spans="1:14">
       <c r="A478" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B478" t="s"/>
       <c r="C478" t="s"/>
@@ -13116,7 +13113,7 @@
     </row>
     <row r="479" spans="1:14">
       <c r="A479" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B479" t="s"/>
       <c r="C479" t="s"/>
@@ -13134,7 +13131,7 @@
     </row>
     <row r="480" spans="1:14">
       <c r="A480" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B480" t="s"/>
       <c r="C480" t="s"/>
@@ -13152,7 +13149,7 @@
     </row>
     <row r="481" spans="1:14">
       <c r="A481" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B481" t="s"/>
       <c r="C481" t="s"/>

</xml_diff>